<commit_message>
Correction + verification du code
</commit_message>
<xml_diff>
--- a/Documentation/Annexe/Journal de bord/Journal_De_Bord.xlsx
+++ b/Documentation/Annexe/Journal de bord/Journal_De_Bord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BatailleNavale\BatailleNavale\Annexe\Journal de bord\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BatailleNavale\BatailleNavale\Documentation\Annexe\Journal de bord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48713896-C2E2-45FB-AAB9-A29B22B5825F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A7D2EF-639F-4D7C-BE77-0661E3E98404}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="2715" windowWidth="28800" windowHeight="15435" xr2:uid="{57B1B7D4-CFAD-40D2-8F45-3ECB3F6C0466}"/>
+    <workbookView xWindow="7245" yWindow="3060" windowWidth="28800" windowHeight="15435" xr2:uid="{57B1B7D4-CFAD-40D2-8F45-3ECB3F6C0466}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Événement</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Fin de la version 1.0</t>
+  </si>
+  <si>
+    <t>Début de la rédaction de la documentation du projet</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,8 +490,12 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="3">
+        <v>43923</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
Mise a jour de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/Annexe/Journal de bord/Journal_De_Bord.xlsx
+++ b/Documentation/Annexe/Journal de bord/Journal_De_Bord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BatailleNavale\BatailleNavale\Documentation\Annexe\Journal de bord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A7D2EF-639F-4D7C-BE77-0661E3E98404}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C998EA8-C418-4221-9710-8320AD314DD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7245" yWindow="3060" windowWidth="28800" windowHeight="15435" xr2:uid="{57B1B7D4-CFAD-40D2-8F45-3ECB3F6C0466}"/>
+    <workbookView xWindow="5850" yWindow="2100" windowWidth="28800" windowHeight="15435" xr2:uid="{57B1B7D4-CFAD-40D2-8F45-3ECB3F6C0466}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Événement</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Début de la rédaction de la documentation du projet</t>
+  </si>
+  <si>
+    <t>Rendu de la version de la version 1.0 du projet et fin du sprint 6</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,8 +501,12 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="3">
+        <v>43929</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>

</xml_diff>